<commit_message>
added BKMP differentiated analysis
</commit_message>
<xml_diff>
--- a/Fragebogen/Fragebogen_Auswertung_quantitativ.xlsx
+++ b/Fragebogen/Fragebogen_Auswertung_quantitativ.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\Uni\BA\Durchführung\Datenanalyse\Fragebogen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Desktop\Uni\BA\Durchführung\Datenanalyse\Fragebogen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1962BBB1-45FE-425A-A798-5FA5DBC1E436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA87379-714F-480E-9EAB-70AE1AE2FE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>TeilnehmerIn</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Standartabweichung</t>
+  </si>
+  <si>
+    <t>revidieren</t>
   </si>
 </sst>
 </file>
@@ -464,18 +467,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="255" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,7 +540,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -597,7 +600,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -659,7 +662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -719,7 +722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -781,7 +784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -843,7 +846,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -905,7 +908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -967,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1027,7 +1030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
@@ -1052,51 +1055,51 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4">
-        <f>AVERAGE(J2:J9)</f>
+        <f t="shared" ref="J10:T10" si="1">AVERAGE(J2:J9)</f>
         <v>3.125</v>
       </c>
       <c r="K10" s="4">
-        <f>AVERAGE(K2:K9)</f>
+        <f t="shared" si="1"/>
         <v>3.375</v>
       </c>
       <c r="L10" s="4">
-        <f>AVERAGE(L2:L9)</f>
+        <f t="shared" si="1"/>
         <v>1.375</v>
       </c>
       <c r="M10" s="4">
-        <f>AVERAGE(M2:M9)</f>
+        <f t="shared" si="1"/>
         <v>1.875</v>
       </c>
       <c r="N10" s="4">
-        <f>AVERAGE(N2:N9)</f>
+        <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
       <c r="O10" s="4">
-        <f>AVERAGE(O2:O9)</f>
+        <f t="shared" si="1"/>
         <v>1.625</v>
       </c>
       <c r="P10" s="4">
-        <f>AVERAGE(P2:P9)</f>
+        <f t="shared" si="1"/>
         <v>3.375</v>
       </c>
       <c r="Q10" s="4">
-        <f>AVERAGE(Q2:Q9)</f>
+        <f t="shared" si="1"/>
         <v>2.375</v>
       </c>
       <c r="R10" s="4">
-        <f>AVERAGE(R2:R9)</f>
+        <f t="shared" si="1"/>
         <v>3.2</v>
       </c>
       <c r="S10" s="4">
-        <f>AVERAGE(S2:S9)</f>
+        <f t="shared" si="1"/>
         <v>3.25</v>
       </c>
       <c r="T10" s="4">
-        <f>AVERAGE(T2:T9)</f>
+        <f t="shared" si="1"/>
         <v>3.75</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
@@ -1106,63 +1109,74 @@
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4">
-        <f t="shared" ref="D11:F11" si="1">_xlfn.STDEV.P(D2:D9)</f>
+        <f t="shared" ref="D11:F11" si="2">_xlfn.STDEV.P(D2:D9)</f>
         <v>12.786100852097171</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.212120707339915</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.176895816785846</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4">
-        <f t="shared" ref="J11:T11" si="2">_xlfn.STDEV.P(J2:J9)</f>
+        <f t="shared" ref="J11:T11" si="3">_xlfn.STDEV.P(J2:J9)</f>
         <v>0.78062474979979979</v>
       </c>
       <c r="K11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.69597054535375269</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.99215674164922152</v>
       </c>
       <c r="M11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.165922381636102</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.66143782776614768</v>
       </c>
       <c r="O11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1110243021644486</v>
       </c>
       <c r="P11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.69597054535375269</v>
       </c>
       <c r="Q11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3169567191065923</v>
       </c>
       <c r="R11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.74833147735478833</v>
       </c>
       <c r="S11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3919410907075054</v>
       </c>
       <c r="T11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.82915619758884995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="L12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>